<commit_message>
Changed prices in main quote system
</commit_message>
<xml_diff>
--- a/local/components/custom/quotation.system/quatation_print.xlsx
+++ b/local/components/custom/quotation.system/quatation_print.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>METAL  PRO BUILDINGS</t>
   </si>
@@ -41,7 +41,7 @@
     <t>Customer ID:</t>
   </si>
   <si>
-    <t>L_111343</t>
+    <t>L_110365</t>
   </si>
   <si>
     <t xml:space="preserve">Customer : </t>
@@ -62,10 +62,10 @@
     <t>Email:</t>
   </si>
   <si>
-    <t>Kent  Chaulk</t>
+    <t>Ben  Jacobson</t>
   </si>
   <si>
-    <t>Inquire@live.ca</t>
+    <t>btb9335@gmail.com</t>
   </si>
   <si>
     <t>Mailing Address:</t>
@@ -80,13 +80,16 @@
     <t>Postal Code:</t>
   </si>
   <si>
+    <t>Grande Prairie</t>
+  </si>
+  <si>
     <t>Building Address:</t>
   </si>
   <si>
-    <t>Labrador City</t>
+    <t>Slave Lake</t>
   </si>
   <si>
-    <t>NL</t>
+    <t>AB</t>
   </si>
   <si>
     <t>Ship to:</t>
@@ -119,16 +122,13 @@
     <t>LOW (CATEGORY I) SHELTERED</t>
   </si>
   <si>
-    <t>S-SERIES</t>
+    <t>MINI</t>
   </si>
   <si>
-    <t>S20-12</t>
+    <t>M14-10</t>
   </si>
   <si>
-    <t>TROUGH</t>
-  </si>
-  <si>
-    <t>22/20</t>
+    <t>CHANNEL</t>
   </si>
   <si>
     <t xml:space="preserve">     Arches</t>
@@ -149,12 +149,6 @@
     <t xml:space="preserve">     Rear Wall</t>
   </si>
   <si>
-    <t>SOLID</t>
-  </si>
-  <si>
-    <t>INCLUDED</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Accessories 
 </t>
   </si>
@@ -173,6 +167,9 @@
   </si>
   <si>
     <t>✔ 110% Nuts &amp; Bolts**</t>
+  </si>
+  <si>
+    <t>INCLUDED</t>
   </si>
   <si>
     <t>Not included</t>
@@ -2383,7 +2380,7 @@
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27">
-        <v>17096972219</v>
+        <v>17804021780</v>
       </c>
       <c r="I8" s="28" t="s">
         <v>16</v>
@@ -2447,7 +2444,9 @@
       <c r="B10" s="31"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
-      <c r="E10" s="216"/>
+      <c r="E10" s="216" t="s">
+        <v>21</v>
+      </c>
       <c r="F10" s="217"/>
       <c r="G10" s="25"/>
       <c r="H10" s="24"/>
@@ -2472,7 +2471,7 @@
     </row>
     <row r="11" spans="1:28" customHeight="1" ht="30">
       <c r="A11" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2512,11 +2511,11 @@
       <c r="C12" s="36"/>
       <c r="D12" s="37"/>
       <c r="E12" s="218" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="219"/>
       <c r="G12" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H12" s="37"/>
       <c r="I12" s="34"/>
@@ -2568,7 +2567,7 @@
     </row>
     <row r="14" spans="1:28" customHeight="1" ht="30">
       <c r="A14" s="38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -2608,11 +2607,11 @@
       <c r="C15" s="36"/>
       <c r="D15" s="37"/>
       <c r="E15" s="218" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="219"/>
       <c r="G15" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H15" s="37"/>
       <c r="I15" s="34"/>
@@ -2664,30 +2663,30 @@
     </row>
     <row r="17" spans="1:28" customHeight="1" ht="35">
       <c r="A17" s="226" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="227"/>
       <c r="C17" s="44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" s="228" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F17" s="229"/>
       <c r="G17" s="45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I17" s="45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K17" s="46"/>
       <c r="L17" s="46"/>
@@ -2708,30 +2707,30 @@
     </row>
     <row r="18" spans="1:28" customHeight="1" ht="71.25">
       <c r="A18" s="230" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="231"/>
       <c r="C18" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E18" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="50">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H18" s="51">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I18" s="52">
-        <v>12</v>
+        <v>10</v>
       </c>
-      <c r="J18" s="52" t="s">
-        <v>37</v>
+      <c r="J18" s="52">
+        <v>22</v>
       </c>
       <c r="K18" s="53"/>
       <c r="L18" s="53"/>
@@ -2759,7 +2758,7 @@
       <c r="D19" s="55"/>
       <c r="E19" s="56">
         <f>IF(C18="MINI",H18/1.5-1,H18/2-1)</f>
-        <v>14</v>
+        <v>16.333333333333</v>
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="57"/>
@@ -2908,20 +2907,20 @@
         <v>42</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F24" s="68"/>
       <c r="G24" s="69" t="s">
         <v>42</v>
       </c>
       <c r="H24" s="67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I24" s="67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J24" s="70"/>
       <c r="K24" s="71"/>
@@ -2977,11 +2976,11 @@
       </c>
       <c r="B26" s="241"/>
       <c r="C26" s="76" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D26" s="79"/>
       <c r="E26" s="245" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F26" s="246"/>
       <c r="G26" s="80"/>
@@ -3012,20 +3011,20 @@
         <v>42</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F27" s="83"/>
       <c r="G27" s="69" t="s">
         <v>42</v>
       </c>
       <c r="H27" s="67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I27" s="67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J27" s="84"/>
       <c r="K27" s="85"/>
@@ -3105,7 +3104,7 @@
     </row>
     <row r="30" spans="1:28" customHeight="1" ht="37.5">
       <c r="A30" s="249" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="250"/>
       <c r="C30" s="250"/>
@@ -3251,7 +3250,7 @@
     </row>
     <row r="35" spans="1:28" customHeight="1" ht="36">
       <c r="A35" s="252" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" s="250"/>
       <c r="C35" s="250"/>
@@ -3288,10 +3287,10 @@
         <v>42</v>
       </c>
       <c r="F36" s="109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G36" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H36" s="110"/>
       <c r="I36" s="111"/>
@@ -3399,20 +3398,20 @@
     </row>
     <row r="40" spans="1:28" customHeight="1" ht="34.5">
       <c r="A40" s="127" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="128"/>
       <c r="C40" s="128"/>
       <c r="D40" s="129"/>
       <c r="E40" s="130"/>
       <c r="F40" s="131" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G40" s="132"/>
       <c r="H40" s="133"/>
       <c r="I40" s="133"/>
       <c r="J40" s="134" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K40" s="107"/>
       <c r="L40" s="107"/>
@@ -3437,16 +3436,16 @@
       <c r="C41" s="135"/>
       <c r="D41" s="135"/>
       <c r="E41" s="136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" s="137" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G41" s="138"/>
       <c r="H41" s="139"/>
       <c r="I41" s="139"/>
       <c r="J41" s="140" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K41" s="72"/>
       <c r="L41" s="72"/>
@@ -3467,20 +3466,20 @@
     </row>
     <row r="42" spans="1:28" customHeight="1" ht="45">
       <c r="A42" s="141" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="142"/>
       <c r="C42" s="143"/>
       <c r="D42" s="144"/>
       <c r="E42" s="145"/>
       <c r="F42" s="146" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G42" s="146"/>
       <c r="H42" s="147"/>
       <c r="I42" s="147"/>
       <c r="J42" s="148" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K42" s="149"/>
       <c r="L42" s="149"/>
@@ -3529,14 +3528,14 @@
     </row>
     <row r="44" spans="1:28" customHeight="1" ht="68.25">
       <c r="A44" s="150" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="151"/>
       <c r="C44" s="152"/>
       <c r="D44" s="152"/>
       <c r="E44" s="153"/>
       <c r="F44" s="253" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G44" s="254"/>
       <c r="H44" s="254"/>
@@ -3561,13 +3560,13 @@
     </row>
     <row r="45" spans="1:28" customHeight="1" ht="35.25">
       <c r="A45" s="154" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="155"/>
       <c r="C45" s="156"/>
       <c r="D45" s="156"/>
       <c r="E45" s="157" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F45" s="225"/>
       <c r="G45" s="225"/>
@@ -3711,7 +3710,7 @@
       <c r="E50" s="169"/>
       <c r="F50" s="169"/>
       <c r="G50" s="204" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H50" s="205"/>
       <c r="I50" s="205"/>
@@ -3741,12 +3740,12 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="209" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H51" s="210"/>
       <c r="I51" s="211"/>
       <c r="J51" s="172">
-        <v>21698.496923077</v>
+        <v>17280.389082517</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -3773,12 +3772,12 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="206" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H52" s="207"/>
       <c r="I52" s="208"/>
       <c r="J52" s="173">
-        <v>6000.0</v>
+        <v>6750.0</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -3808,7 +3807,7 @@
       <c r="H53" s="177"/>
       <c r="I53" s="178"/>
       <c r="J53" s="179">
-        <v>27698.496923077</v>
+        <v>24030.389082517</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -3913,18 +3912,18 @@
     </row>
     <row r="57" spans="1:28" customHeight="1" ht="26.25">
       <c r="A57" s="186" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="180"/>
       <c r="C57" s="66" t="str">
         <f>$A$8&amp;" "&amp;$E$8</f>
-        <v>Kent  Chaulk </v>
+        <v>Ben  Jacobson </v>
       </c>
       <c r="D57" s="181"/>
       <c r="E57" s="181"/>
       <c r="F57" s="181"/>
       <c r="G57" s="187" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H57" s="180"/>
       <c r="I57" s="182"/>
@@ -3954,7 +3953,7 @@
       <c r="E58" s="181"/>
       <c r="F58" s="181"/>
       <c r="G58" s="184" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H58" s="180"/>
       <c r="I58" s="182"/>
@@ -4118,13 +4117,13 @@
     </row>
     <row r="64" spans="1:28" customHeight="1" ht="15.75">
       <c r="A64" s="193" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -4178,7 +4177,7 @@
     </row>
     <row r="66" spans="1:28" customHeight="1" ht="63">
       <c r="A66" s="260" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="261"/>
       <c r="C66" s="261"/>
@@ -4208,7 +4207,7 @@
     </row>
     <row r="67" spans="1:28" customHeight="1" ht="33">
       <c r="A67" s="263" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" s="264"/>
       <c r="C67" s="264"/>
@@ -4238,7 +4237,7 @@
     </row>
     <row r="68" spans="1:28" customHeight="1" ht="32">
       <c r="A68" s="263" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" s="264"/>
       <c r="C68" s="264"/>
@@ -4268,7 +4267,7 @@
     </row>
     <row r="69" spans="1:28" customHeight="1" ht="48">
       <c r="A69" s="263" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="264"/>
       <c r="C69" s="264"/>
@@ -4298,7 +4297,7 @@
     </row>
     <row r="70" spans="1:28" customHeight="1" ht="30">
       <c r="A70" s="266" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" s="267"/>
       <c r="C70" s="267"/>
@@ -4328,7 +4327,7 @@
     </row>
     <row r="71" spans="1:28" customHeight="1" ht="66">
       <c r="A71" s="266" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="267"/>
       <c r="C71" s="267"/>
@@ -4358,7 +4357,7 @@
     </row>
     <row r="72" spans="1:28" customHeight="1" ht="64">
       <c r="A72" s="266" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" s="267"/>
       <c r="C72" s="267"/>
@@ -4388,7 +4387,7 @@
     </row>
     <row r="73" spans="1:28" customHeight="1" ht="30">
       <c r="A73" s="266" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="267"/>
       <c r="C73" s="267"/>
@@ -4418,7 +4417,7 @@
     </row>
     <row r="74" spans="1:28" customHeight="1" ht="18">
       <c r="A74" s="266" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="267"/>
       <c r="C74" s="267"/>
@@ -4448,7 +4447,7 @@
     </row>
     <row r="75" spans="1:28" customHeight="1" ht="33">
       <c r="A75" s="266" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="267"/>
       <c r="C75" s="267"/>
@@ -4478,7 +4477,7 @@
     </row>
     <row r="76" spans="1:28" customHeight="1" ht="31">
       <c r="A76" s="266" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="267"/>
       <c r="C76" s="267"/>
@@ -4508,7 +4507,7 @@
     </row>
     <row r="77" spans="1:28" customHeight="1" ht="18">
       <c r="A77" s="266" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" s="267"/>
       <c r="C77" s="267"/>
@@ -4538,7 +4537,7 @@
     </row>
     <row r="78" spans="1:28" customHeight="1" ht="17">
       <c r="A78" s="266" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" s="267"/>
       <c r="C78" s="267"/>
@@ -4568,7 +4567,7 @@
     </row>
     <row r="79" spans="1:28" customHeight="1" ht="32">
       <c r="A79" s="266" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="267"/>
       <c r="C79" s="267"/>
@@ -4598,7 +4597,7 @@
     </row>
     <row r="80" spans="1:28" customHeight="1" ht="48">
       <c r="A80" s="266" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" s="267"/>
       <c r="C80" s="267"/>
@@ -4628,7 +4627,7 @@
     </row>
     <row r="81" spans="1:28" customHeight="1" ht="17">
       <c r="A81" s="266" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" s="267"/>
       <c r="C81" s="267"/>
@@ -4658,7 +4657,7 @@
     </row>
     <row r="82" spans="1:28" customHeight="1" ht="50">
       <c r="A82" s="266" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" s="267"/>
       <c r="C82" s="267"/>
@@ -4688,7 +4687,7 @@
     </row>
     <row r="83" spans="1:28" customHeight="1" ht="17">
       <c r="A83" s="266" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" s="267"/>
       <c r="C83" s="267"/>
@@ -4718,7 +4717,7 @@
     </row>
     <row r="84" spans="1:28" customHeight="1" ht="32">
       <c r="A84" s="266" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" s="267"/>
       <c r="C84" s="267"/>
@@ -4748,7 +4747,7 @@
     </row>
     <row r="85" spans="1:28" customHeight="1" ht="32">
       <c r="A85" s="266" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85" s="267"/>
       <c r="C85" s="267"/>
@@ -4778,7 +4777,7 @@
     </row>
     <row r="86" spans="1:28" customHeight="1" ht="23">
       <c r="A86" s="266" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" s="267"/>
       <c r="C86" s="267"/>
@@ -4808,7 +4807,7 @@
     </row>
     <row r="87" spans="1:28" customHeight="1" ht="17">
       <c r="A87" s="266" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87" s="267"/>
       <c r="C87" s="267"/>
@@ -4838,7 +4837,7 @@
     </row>
     <row r="88" spans="1:28" customHeight="1" ht="16" s="201" customFormat="1">
       <c r="A88" s="266" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" s="267"/>
       <c r="C88" s="267"/>
@@ -4868,7 +4867,7 @@
     </row>
     <row r="89" spans="1:28" customHeight="1" ht="19">
       <c r="A89" s="266" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" s="267"/>
       <c r="C89" s="267"/>
@@ -4898,7 +4897,7 @@
     </row>
     <row r="90" spans="1:28" customHeight="1" ht="18">
       <c r="A90" s="266" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" s="267"/>
       <c r="C90" s="267"/>
@@ -4928,7 +4927,7 @@
     </row>
     <row r="91" spans="1:28" customHeight="1" ht="31">
       <c r="A91" s="266" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" s="267"/>
       <c r="C91" s="267"/>
@@ -4958,7 +4957,7 @@
     </row>
     <row r="92" spans="1:28" customHeight="1" ht="34.5">
       <c r="A92" s="266" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" s="267"/>
       <c r="C92" s="267"/>
@@ -4988,7 +4987,7 @@
     </row>
     <row r="93" spans="1:28" customHeight="1" ht="31">
       <c r="A93" s="266" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B93" s="267"/>
       <c r="C93" s="267"/>
@@ -5018,7 +5017,7 @@
     </row>
     <row r="94" spans="1:28" customHeight="1" ht="32">
       <c r="A94" s="266" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" s="267"/>
       <c r="C94" s="267"/>
@@ -5048,7 +5047,7 @@
     </row>
     <row r="95" spans="1:28" customHeight="1" ht="18">
       <c r="A95" s="266" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" s="267"/>
       <c r="C95" s="267"/>
@@ -5078,7 +5077,7 @@
     </row>
     <row r="96" spans="1:28" customHeight="1" ht="51">
       <c r="A96" s="266" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" s="267"/>
       <c r="C96" s="267"/>
@@ -5108,7 +5107,7 @@
     </row>
     <row r="97" spans="1:28" customHeight="1" ht="18">
       <c r="A97" s="266" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B97" s="267"/>
       <c r="C97" s="267"/>
@@ -5138,7 +5137,7 @@
     </row>
     <row r="98" spans="1:28" customHeight="1" ht="33">
       <c r="A98" s="266" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B98" s="267"/>
       <c r="C98" s="267"/>
@@ -5168,7 +5167,7 @@
     </row>
     <row r="99" spans="1:28" customHeight="1" ht="33">
       <c r="A99" s="266" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B99" s="267"/>
       <c r="C99" s="267"/>
@@ -5198,7 +5197,7 @@
     </row>
     <row r="100" spans="1:28" customHeight="1" ht="35">
       <c r="A100" s="266" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B100" s="267"/>
       <c r="C100" s="267"/>
@@ -5228,7 +5227,7 @@
     </row>
     <row r="101" spans="1:28" customHeight="1" ht="46">
       <c r="A101" s="274" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" s="267"/>
       <c r="C101" s="267"/>
@@ -5258,7 +5257,7 @@
     </row>
     <row r="102" spans="1:28" customHeight="1" ht="26" s="201" customFormat="1">
       <c r="A102" s="271" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B102" s="271"/>
       <c r="C102" s="271"/>

</xml_diff>